<commit_message>
Playing around with Acer comparisons
</commit_message>
<xml_diff>
--- a/ED50/Comparison_Acer_Mote_Genets_ED50_djb.xlsx
+++ b/ED50/Comparison_Acer_Mote_Genets_ED50_djb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danbarshis/dansstuff/Projeks/ODU/Projeks/Field/2021_Keys/2021-June_Mote/ED50/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ABB813B5-3D1F-304C-8500-24CC47C955F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0AF85CF-76D6-BA40-89A6-BBFC95FEA3C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1720" yWindow="5460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1720" yWindow="5460" windowWidth="21580" windowHeight="9880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>Genotype</t>
   </si>
@@ -97,6 +97,15 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>USvsRossRank</t>
+  </si>
+  <si>
+    <t>RossCKRank</t>
+  </si>
+  <si>
+    <t>RossvsCKRank</t>
   </si>
 </sst>
 </file>
@@ -483,15 +492,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="15" max="15" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -526,101 +538,108 @@
         <v>18</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B2">
-        <v>35.700000000000003</v>
+        <v>35.32</v>
       </c>
       <c r="C2">
-        <v>34.591763838331907</v>
+        <v>35.041648927661313</v>
       </c>
       <c r="D2">
-        <v>34.953507220980583</v>
+        <v>34.958690306932233</v>
       </c>
       <c r="E2">
-        <v>35.100241493691627</v>
+        <v>35.118889856035992</v>
       </c>
       <c r="F2">
-        <v>34.86</v>
-      </c>
-      <c r="G2">
-        <v>34.08</v>
-      </c>
-      <c r="H2">
-        <f>F2-G2</f>
-        <v>0.78000000000000114</v>
+        <v>35.04</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
       </c>
       <c r="I2">
         <f>B2-F2</f>
-        <v>0.84000000000000341</v>
-      </c>
-      <c r="J2">
-        <f>B2-G2</f>
-        <v>1.6200000000000045</v>
+        <v>0.28000000000000114</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
       </c>
       <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>5</v>
+      </c>
+      <c r="O2">
+        <f>ABS(N2-K2)</f>
         <v>4</v>
       </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <v>2</v>
-      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3">
-        <v>36.049999999999997</v>
+        <v>35.44</v>
       </c>
       <c r="C3">
-        <v>34.993947774642372</v>
+        <v>35.86397961687468</v>
       </c>
       <c r="D3">
-        <v>35.038547593143392</v>
+        <v>35.397433861683119</v>
       </c>
       <c r="E3">
-        <v>34.990568704528577</v>
+        <v>35.396671676446111</v>
       </c>
       <c r="F3">
-        <v>34.979999999999997</v>
-      </c>
-      <c r="G3">
-        <v>34.119999999999997</v>
-      </c>
-      <c r="H3">
-        <f>F3-G3</f>
-        <v>0.85999999999999943</v>
+        <v>35.590000000000003</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
       </c>
       <c r="I3">
         <f>B3-F3</f>
-        <v>1.0700000000000003</v>
-      </c>
-      <c r="J3">
-        <f>B3-G3</f>
-        <v>1.9299999999999997</v>
+        <v>-0.15000000000000568</v>
+      </c>
+      <c r="J3" t="s">
+        <v>21</v>
       </c>
       <c r="K3">
-        <v>7</v>
-      </c>
-      <c r="L3">
         <v>2</v>
       </c>
-      <c r="M3">
-        <v>4</v>
+      <c r="N3">
+        <v>8</v>
+      </c>
+      <c r="O3">
+        <f>ABS(N3-K3)</f>
+        <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -658,196 +677,261 @@
         <v>3</v>
       </c>
       <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
         <v>3</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>1</v>
       </c>
+      <c r="O4">
+        <f>ABS(N4-K4)</f>
+        <v>2</v>
+      </c>
+      <c r="P4">
+        <f>ABS(L4-M4)</f>
+        <v>2</v>
+      </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>35.92</v>
+        <v>35.700000000000003</v>
       </c>
       <c r="C5">
-        <v>35.438582785050869</v>
+        <v>34.591763838331907</v>
       </c>
       <c r="D5">
-        <v>35.322826342416931</v>
+        <v>34.953507220980583</v>
       </c>
       <c r="E5">
-        <v>35.353823343265262</v>
+        <v>35.100241493691627</v>
       </c>
       <c r="F5">
-        <v>35.520000000000003</v>
+        <v>34.86</v>
       </c>
       <c r="G5">
-        <v>34.520000000000003</v>
+        <v>34.08</v>
       </c>
       <c r="H5">
         <f>F5-G5</f>
-        <v>1</v>
+        <v>0.78000000000000114</v>
       </c>
       <c r="I5">
         <f>B5-F5</f>
-        <v>0.39999999999999858</v>
+        <v>0.84000000000000341</v>
       </c>
       <c r="J5">
         <f>B5-G5</f>
-        <v>1.3999999999999986</v>
+        <v>1.6200000000000045</v>
       </c>
       <c r="K5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M5">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>2</v>
+      </c>
+      <c r="O5">
+        <f>ABS(N5-K5)</f>
+        <v>2</v>
+      </c>
+      <c r="P5">
+        <f t="shared" ref="P5:P8" si="0">ABS(L5-M5)</f>
+        <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B6">
-        <v>35.94</v>
+        <v>35.92</v>
       </c>
       <c r="C6">
-        <v>35.159331124142803</v>
+        <v>35.438582785050869</v>
       </c>
       <c r="D6">
-        <v>35.236710507767768</v>
+        <v>35.322826342416931</v>
       </c>
       <c r="E6">
-        <v>36.154395883287208</v>
+        <v>35.353823343265262</v>
       </c>
       <c r="F6">
-        <v>35.44</v>
+        <v>35.520000000000003</v>
       </c>
       <c r="G6">
-        <v>34.659999999999997</v>
+        <v>34.520000000000003</v>
       </c>
       <c r="H6">
         <f>F6-G6</f>
-        <v>0.78000000000000114</v>
+        <v>1</v>
       </c>
       <c r="I6">
         <f>B6-F6</f>
-        <v>0.5</v>
+        <v>0.39999999999999858</v>
       </c>
       <c r="J6">
         <f>B6-G6</f>
-        <v>1.2800000000000011</v>
+        <v>1.3999999999999986</v>
       </c>
       <c r="K6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L6">
+        <v>3</v>
+      </c>
+      <c r="M6">
+        <v>4</v>
+      </c>
+      <c r="N6">
+        <v>7</v>
+      </c>
+      <c r="O6">
+        <f>ABS(N6-K6)</f>
+        <v>2</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="M6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
       <c r="B7">
-        <v>36.42</v>
+        <v>35.94</v>
       </c>
       <c r="C7">
-        <v>35.018540865958848</v>
+        <v>35.159331124142803</v>
       </c>
       <c r="D7">
-        <v>34.938776119327351</v>
+        <v>35.236710507767768</v>
       </c>
       <c r="E7">
-        <v>34.902855976402861</v>
+        <v>36.154395883287208</v>
       </c>
       <c r="F7">
-        <v>34.94</v>
-      </c>
-      <c r="G7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" t="s">
-        <v>21</v>
+        <v>35.44</v>
+      </c>
+      <c r="G7">
+        <v>34.659999999999997</v>
+      </c>
+      <c r="H7">
+        <f>F7-G7</f>
+        <v>0.78000000000000114</v>
       </c>
       <c r="I7">
         <f>B7-F7</f>
-        <v>1.480000000000004</v>
-      </c>
-      <c r="J7" t="s">
-        <v>21</v>
+        <v>0.5</v>
+      </c>
+      <c r="J7">
+        <f>B7-G7</f>
+        <v>1.2800000000000011</v>
       </c>
       <c r="K7">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="L7">
+        <v>4</v>
       </c>
       <c r="M7">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="N7">
+        <v>6</v>
+      </c>
+      <c r="O7">
+        <f>ABS(N7-K7)</f>
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8">
-        <v>35.32</v>
+        <v>36.049999999999997</v>
       </c>
       <c r="C8">
-        <v>35.041648927661313</v>
+        <v>34.993947774642372</v>
       </c>
       <c r="D8">
-        <v>34.958690306932233</v>
+        <v>35.038547593143392</v>
       </c>
       <c r="E8">
-        <v>35.118889856035992</v>
+        <v>34.990568704528577</v>
       </c>
       <c r="F8">
-        <v>35.04</v>
-      </c>
-      <c r="G8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" t="s">
-        <v>21</v>
+        <v>34.979999999999997</v>
+      </c>
+      <c r="G8">
+        <v>34.119999999999997</v>
+      </c>
+      <c r="H8">
+        <f>F8-G8</f>
+        <v>0.85999999999999943</v>
       </c>
       <c r="I8">
         <f>B8-F8</f>
-        <v>0.28000000000000114</v>
-      </c>
-      <c r="J8" t="s">
-        <v>21</v>
+        <v>1.0700000000000003</v>
+      </c>
+      <c r="J8">
+        <f>B8-G8</f>
+        <v>1.9299999999999997</v>
       </c>
       <c r="K8">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="L8">
+        <v>5</v>
       </c>
       <c r="M8">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="N8">
+        <v>4</v>
+      </c>
+      <c r="O8">
+        <f>ABS(N8-K8)</f>
+        <v>3</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>35.44</v>
+        <v>36.42</v>
       </c>
       <c r="C9">
-        <v>35.86397961687468</v>
+        <v>35.018540865958848</v>
       </c>
       <c r="D9">
-        <v>35.397433861683119</v>
+        <v>34.938776119327351</v>
       </c>
       <c r="E9">
-        <v>35.396671676446111</v>
+        <v>34.902855976402861</v>
       </c>
       <c r="F9">
-        <v>35.590000000000003</v>
+        <v>34.94</v>
       </c>
       <c r="G9" t="s">
         <v>21</v>
@@ -857,22 +941,38 @@
       </c>
       <c r="I9">
         <f>B9-F9</f>
-        <v>-0.15000000000000568</v>
+        <v>1.480000000000004</v>
       </c>
       <c r="J9" t="s">
         <v>21</v>
       </c>
       <c r="K9">
-        <v>2</v>
-      </c>
-      <c r="M9">
         <v>8</v>
       </c>
+      <c r="N9">
+        <v>3</v>
+      </c>
+      <c r="O9">
+        <f>ABS(N9-K9)</f>
+        <v>5</v>
+      </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <f>MAX(B2:B9)-MIN(B2:B9)</f>
+        <v>1.1000000000000014</v>
+      </c>
+      <c r="F10">
+        <f>MAX(F2:F9)-MIN(F2:F9)</f>
+        <v>0.8300000000000054</v>
+      </c>
+      <c r="G10">
+        <f>MAX(G2:G9)-MIN(G2:G9)</f>
+        <v>0.57999999999999829</v>
+      </c>
       <c r="H10">
         <f>AVERAGE(H2:H6)</f>
-        <v>0.79000000000000059</v>
+        <v>0.77000000000000079</v>
       </c>
       <c r="I10">
         <f>AVERAGE(I2:I9)</f>
@@ -880,12 +980,20 @@
       </c>
       <c r="J10">
         <f>AVERAGE(J2:J6)</f>
-        <v>1.5280000000000016</v>
+        <v>1.476666666666669</v>
+      </c>
+      <c r="O10">
+        <f>AVERAGE(O2:O9)</f>
+        <v>3</v>
+      </c>
+      <c r="P10">
+        <f>AVERAGE(P4:P8)</f>
+        <v>1.6</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M9">
-    <sortCondition ref="G2:G9"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O9">
+    <sortCondition ref="B2:B9"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>